<commit_message>
mtcars Excel updates - Correlation - Linear Regression
</commit_message>
<xml_diff>
--- a/Intro to Statistics/mtcars.xlsx
+++ b/Intro to Statistics/mtcars.xlsx
@@ -1,26 +1,71 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eskim\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Online Learning\DataRockie Bootcamp\DataRockie Bootcamp 10th\Intro to Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A8C4B35-D717-41B7-9ADF-8073591CC4F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3F4F95-6259-4328-BCFA-66DDA9FD8F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mtcars" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">mtcars!$M$4</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
   <si>
     <t>mpg</t>
   </si>
@@ -53,13 +98,170 @@
   </si>
   <si>
     <t>carb</t>
+  </si>
+  <si>
+    <t>Correlation Matrix</t>
+  </si>
+  <si>
+    <t>mpg = f(hp)</t>
+  </si>
+  <si>
+    <t>mpg = b0 +b1*hp</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
+  </si>
+  <si>
+    <t>Corr</t>
+  </si>
+  <si>
+    <t>Corr ^ 2</t>
+  </si>
+  <si>
+    <t>&lt; 0.05</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t>=&gt;&gt; Significance</t>
+  </si>
+  <si>
+    <t>Explained Variances</t>
+  </si>
+  <si>
+    <t>Overall Significance of the Model</t>
+  </si>
+  <si>
+    <t>MPG = 30.10 + ( -0.07 * hp)</t>
+  </si>
+  <si>
+    <t>ex. hp = 200</t>
+  </si>
+  <si>
+    <t>Predicted MPG</t>
+  </si>
+  <si>
+    <t>Confidence Interval</t>
+  </si>
+  <si>
+    <t>mpg = f(hp, wt, am)</t>
+  </si>
+  <si>
+    <t>mpg = b0 + b1*hp + b2*wt + b3*am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is at least 1 significance parameters which can predict y or mpg </t>
+  </si>
+  <si>
+    <t>MPG = 34.0029 + (-0.0374*hp) + (-2.8785*wt) + (2.0837*am)</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>1 = Manual</t>
+  </si>
+  <si>
+    <t>0 = Auto</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>1. Prediction</t>
+  </si>
+  <si>
+    <t>2. Inference (Why)</t>
+  </si>
+  <si>
+    <t>Corr (actual y, predicted y)</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +396,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,8 +585,38 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -491,6 +731,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -536,8 +796,58 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -583,7 +893,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -596,10 +914,1232 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scatter plot: hp vs mpg</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>mtcars!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mpg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>mtcars!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>mtcars!$B$2:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>32.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>33.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30.4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8B6-4A76-9998-13EEDF5A2F19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1204620383"/>
+        <c:axId val="1204627103"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1204620383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>hp</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1204627103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1204627103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>miles per gallon</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1204620383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>430530</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>163830</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C71A41B4-A57B-1CE9-C580-08AABB99BDAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -637,7 +2177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -743,7 +2283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -885,32 +2425,47 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="13" max="13" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.109375" customWidth="1"/>
+    <col min="28" max="28" width="11.109375" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" customWidth="1"/>
+    <col min="30" max="30" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5546875" customWidth="1"/>
+    <col min="32" max="32" width="12" customWidth="1"/>
+    <col min="33" max="33" width="11.5546875" customWidth="1"/>
+    <col min="34" max="34" width="12.21875" customWidth="1"/>
+    <col min="35" max="35" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -934,18 +2489,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2">
         <v>21</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>160</v>
-      </c>
-      <c r="D2">
-        <v>110</v>
       </c>
       <c r="E2">
         <v>3.9</v>
@@ -968,19 +2523,28 @@
       <c r="K2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M2" s="8">
+        <f>CORREL(B2:B33,A2:A33)</f>
+        <v>-0.77616837182658638</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="U2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3">
+        <v>110</v>
+      </c>
+      <c r="B3">
         <v>21</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>160</v>
-      </c>
-      <c r="D3">
-        <v>110</v>
       </c>
       <c r="E3">
         <v>3.9</v>
@@ -1003,19 +2567,28 @@
       <c r="K3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="U3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>93</v>
+      </c>
+      <c r="B4">
         <v>22.8</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>108</v>
-      </c>
-      <c r="D4">
-        <v>93</v>
       </c>
       <c r="E4">
         <v>3.85</v>
@@ -1038,19 +2611,26 @@
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M4" s="10"/>
+      <c r="N4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5">
         <v>21.4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>258</v>
-      </c>
-      <c r="D5">
-        <v>110</v>
       </c>
       <c r="E5">
         <v>3.08</v>
@@ -1073,19 +2653,41 @@
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="15">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="U5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="17">
+        <f>INTERCEPT($B$2:$B$33,$A$2:$A$33)</f>
+        <v>30.098860539622493</v>
+      </c>
+      <c r="W5" s="16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(V5)</f>
+        <v>=INTERCEPT($B$2:$B$33,$A$2:$A$33)</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="18"/>
+    </row>
+    <row r="6" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>175</v>
+      </c>
+      <c r="B6">
         <v>18.7</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>360</v>
-      </c>
-      <c r="D6">
-        <v>175</v>
       </c>
       <c r="E6">
         <v>3.15</v>
@@ -1108,19 +2710,52 @@
       <c r="K6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="11">
+        <v>-0.77616837182658638</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="17">
+        <f>SLOPE($B$2:$B$33,$A$2:$A$33)</f>
+        <v>-6.8228278071563661E-2</v>
+      </c>
+      <c r="W6" s="16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(V6)</f>
+        <v>=SLOPE($B$2:$B$33,$A$2:$A$33)</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB6" s="6">
+        <v>0.77616837182658638</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE6" s="12">
+        <f>CORREL(B2:B33,A2:A33)</f>
+        <v>-0.77616837182658638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7">
         <v>18.100000000000001</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>225</v>
-      </c>
-      <c r="D7">
-        <v>105</v>
       </c>
       <c r="E7">
         <v>2.76</v>
@@ -1143,19 +2778,35 @@
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB7" s="19">
+        <v>0.60243734142393413</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE7" s="12">
+        <f>AE6^2</f>
+        <v>0.60243734142393401</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>245</v>
+      </c>
+      <c r="B8">
         <v>14.3</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>8</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>360</v>
-      </c>
-      <c r="D8">
-        <v>245</v>
       </c>
       <c r="E8">
         <v>3.21</v>
@@ -1178,19 +2829,25 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>0.589185252804732</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>62</v>
+      </c>
+      <c r="B9">
         <v>24.4</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>4</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>146.69999999999999</v>
-      </c>
-      <c r="D9">
-        <v>62</v>
       </c>
       <c r="E9">
         <v>3.69</v>
@@ -1213,19 +2870,25 @@
       <c r="K9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>3.8629622206479564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>95</v>
+      </c>
+      <c r="B10">
         <v>22.8</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>140.80000000000001</v>
-      </c>
-      <c r="D10">
-        <v>95</v>
       </c>
       <c r="E10">
         <v>3.92</v>
@@ -1248,19 +2911,25 @@
       <c r="K10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>123</v>
+      </c>
+      <c r="B11">
         <v>19.2</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>167.6</v>
-      </c>
-      <c r="D11">
-        <v>123</v>
       </c>
       <c r="E11">
         <v>3.92</v>
@@ -1284,18 +2953,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
+        <v>123</v>
+      </c>
+      <c r="B12">
         <v>17.8</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>167.6</v>
-      </c>
-      <c r="D12">
-        <v>123</v>
       </c>
       <c r="E12">
         <v>3.92</v>
@@ -1318,19 +2987,25 @@
       <c r="K12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA12" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB12" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
         <v>16.399999999999999</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>275.8</v>
-      </c>
-      <c r="D13">
-        <v>180</v>
       </c>
       <c r="E13">
         <v>3.07</v>
@@ -1353,19 +3028,35 @@
       <c r="K13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA13" s="3"/>
+      <c r="AB13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>180</v>
+      </c>
+      <c r="B14">
         <v>17.3</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>275.8</v>
-      </c>
-      <c r="D14">
-        <v>180</v>
       </c>
       <c r="E14">
         <v>3.07</v>
@@ -1388,19 +3079,43 @@
       <c r="K14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="6">
+        <v>678.37287395539829</v>
+      </c>
+      <c r="AD14" s="6">
+        <v>678.37287395539829</v>
+      </c>
+      <c r="AE14" s="6">
+        <v>45.459803260823819</v>
+      </c>
+      <c r="AF14" s="20">
+        <v>1.7878352541210598E-7</v>
+      </c>
+      <c r="AG14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH14" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15">
+        <v>180</v>
+      </c>
+      <c r="B15">
         <v>15.2</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>8</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>275.8</v>
-      </c>
-      <c r="D15">
-        <v>180</v>
       </c>
       <c r="E15">
         <v>3.07</v>
@@ -1423,19 +3138,33 @@
       <c r="K15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB15" s="1">
+        <v>30</v>
+      </c>
+      <c r="AC15" s="6">
+        <v>447.67431354460172</v>
+      </c>
+      <c r="AD15" s="6">
+        <v>14.92247711815339</v>
+      </c>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+    </row>
+    <row r="16" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>205</v>
+      </c>
+      <c r="B16">
         <v>10.4</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>8</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>472</v>
-      </c>
-      <c r="D16">
-        <v>205</v>
       </c>
       <c r="E16">
         <v>2.93</v>
@@ -1458,19 +3187,31 @@
       <c r="K16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>31</v>
+      </c>
+      <c r="AC16" s="7">
+        <v>1126.0471875000001</v>
+      </c>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
+        <v>215</v>
+      </c>
+      <c r="B17">
         <v>10.4</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>8</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>460</v>
-      </c>
-      <c r="D17">
-        <v>215</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1493,19 +3234,25 @@
       <c r="K17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AF17" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG17" s="26"/>
+      <c r="AH17" s="26"/>
+      <c r="AI17" s="26"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18">
+        <v>230</v>
+      </c>
+      <c r="B18">
         <v>14.7</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>8</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>440</v>
-      </c>
-      <c r="D18">
-        <v>230</v>
       </c>
       <c r="E18">
         <v>3.23</v>
@@ -1528,19 +3275,44 @@
       <c r="K18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19">
+        <v>66</v>
+      </c>
+      <c r="B19">
         <v>32.4</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>78.7</v>
-      </c>
-      <c r="D19">
-        <v>66</v>
       </c>
       <c r="E19">
         <v>4.08</v>
@@ -1563,19 +3335,46 @@
       <c r="K19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB19" s="20">
+        <v>30.098860539622493</v>
+      </c>
+      <c r="AC19" s="6">
+        <v>1.633920950302906</v>
+      </c>
+      <c r="AD19" s="6">
+        <v>18.421246470976815</v>
+      </c>
+      <c r="AE19" s="20">
+        <v>6.6427360304650858E-18</v>
+      </c>
+      <c r="AF19" s="6">
+        <v>26.761948787045323</v>
+      </c>
+      <c r="AG19" s="6">
+        <v>33.435772292199658</v>
+      </c>
+      <c r="AH19" s="6">
+        <v>26.761948787045323</v>
+      </c>
+      <c r="AI19" s="6">
+        <v>33.435772292199658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
+        <v>52</v>
+      </c>
+      <c r="B20">
         <v>30.4</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>4</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>75.7</v>
-      </c>
-      <c r="D20">
-        <v>52</v>
       </c>
       <c r="E20">
         <v>4.93</v>
@@ -1598,19 +3397,46 @@
       <c r="K20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA20" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="21">
+        <v>-6.8228278071563689E-2</v>
+      </c>
+      <c r="AC20" s="7">
+        <v>1.0119303810422772E-2</v>
+      </c>
+      <c r="AD20" s="7">
+        <v>-6.7423885427067924</v>
+      </c>
+      <c r="AE20" s="21">
+        <v>1.7878352541210566E-7</v>
+      </c>
+      <c r="AF20" s="21">
+        <v>-8.8894653520534272E-2</v>
+      </c>
+      <c r="AG20" s="21">
+        <v>-4.7561902622593098E-2</v>
+      </c>
+      <c r="AH20" s="21">
+        <v>-8.8894653520534272E-2</v>
+      </c>
+      <c r="AI20" s="21">
+        <v>-4.7561902622593098E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>65</v>
+      </c>
+      <c r="B21">
         <v>33.9</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>71.099999999999994</v>
-      </c>
-      <c r="D21">
-        <v>65</v>
       </c>
       <c r="E21">
         <v>4.22</v>
@@ -1634,18 +3460,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>97</v>
+      </c>
+      <c r="B22">
         <v>21.5</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>120.1</v>
-      </c>
-      <c r="D22">
-        <v>97</v>
       </c>
       <c r="E22">
         <v>3.7</v>
@@ -1668,19 +3494,22 @@
       <c r="K22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23">
+        <v>150</v>
+      </c>
+      <c r="B23">
         <v>15.5</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>8</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>318</v>
-      </c>
-      <c r="D23">
-        <v>150</v>
       </c>
       <c r="E23">
         <v>2.76</v>
@@ -1704,18 +3533,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24">
+        <v>150</v>
+      </c>
+      <c r="B24">
         <v>15.2</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>8</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>304</v>
-      </c>
-      <c r="D24">
-        <v>150</v>
       </c>
       <c r="E24">
         <v>3.15</v>
@@ -1738,19 +3567,22 @@
       <c r="K24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="AA24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25">
+        <v>245</v>
+      </c>
+      <c r="B25">
         <v>13.3</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>8</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>350</v>
-      </c>
-      <c r="D25">
-        <v>245</v>
       </c>
       <c r="E25">
         <v>3.73</v>
@@ -1773,19 +3605,29 @@
       <c r="K25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA25" s="25">
+        <f>AB19+(AB20*200)</f>
+        <v>16.453204925309755</v>
+      </c>
+      <c r="AB25" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A26">
+        <v>175</v>
+      </c>
+      <c r="B26">
         <v>19.2</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>8</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>400</v>
-      </c>
-      <c r="D26">
-        <v>175</v>
       </c>
       <c r="E26">
         <v>3.08</v>
@@ -1808,19 +3650,53 @@
       <c r="K26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M26" s="3"/>
+      <c r="N26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A27">
+        <v>66</v>
+      </c>
+      <c r="B27">
         <v>27.3</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>4</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>79</v>
-      </c>
-      <c r="D27">
-        <v>66</v>
       </c>
       <c r="E27">
         <v>4.08</v>
@@ -1843,19 +3719,33 @@
       <c r="K27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28">
+        <v>91</v>
+      </c>
+      <c r="B28">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>4</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>120.3</v>
-      </c>
-      <c r="D28">
-        <v>91</v>
       </c>
       <c r="E28">
         <v>4.43</v>
@@ -1878,19 +3768,35 @@
       <c r="K28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
+        <v>-0.77616837182658638</v>
+      </c>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+      <c r="X28" s="6"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29">
+        <v>113</v>
+      </c>
+      <c r="B29">
         <v>30.4</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>4</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>95.1</v>
-      </c>
-      <c r="D29">
-        <v>113</v>
       </c>
       <c r="E29">
         <v>3.77</v>
@@ -1913,19 +3819,37 @@
       <c r="K29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" s="6">
+        <v>0.83244745272181953</v>
+      </c>
+      <c r="O29" s="6">
+        <v>-0.8521619594266131</v>
+      </c>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30">
+        <v>264</v>
+      </c>
+      <c r="B30">
         <v>15.8</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>8</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>351</v>
-      </c>
-      <c r="D30">
-        <v>264</v>
       </c>
       <c r="E30">
         <v>4.22</v>
@@ -1948,19 +3872,39 @@
       <c r="K30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N30" s="6">
+        <v>0.79094858636980647</v>
+      </c>
+      <c r="O30" s="6">
+        <v>-0.84755137926247848</v>
+      </c>
+      <c r="P30" s="6">
+        <v>0.9020328721469989</v>
+      </c>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+      <c r="X30" s="6"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31">
+        <v>175</v>
+      </c>
+      <c r="B31">
         <v>19.7</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>6</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>145</v>
-      </c>
-      <c r="D31">
-        <v>175</v>
       </c>
       <c r="E31">
         <v>3.62</v>
@@ -1983,19 +3927,41 @@
       <c r="K31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="6">
+        <v>-0.44875911687291947</v>
+      </c>
+      <c r="O31" s="6">
+        <v>0.68117190780674908</v>
+      </c>
+      <c r="P31" s="6">
+        <v>-0.69993811382876991</v>
+      </c>
+      <c r="Q31" s="6">
+        <v>-0.71021392716927001</v>
+      </c>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+      <c r="X31" s="6"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32">
+        <v>335</v>
+      </c>
+      <c r="B32">
         <v>15</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>8</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>301</v>
-      </c>
-      <c r="D32">
-        <v>335</v>
       </c>
       <c r="E32">
         <v>3.54</v>
@@ -2018,19 +3984,43 @@
       <c r="K32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="M32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0.6587478873447592</v>
+      </c>
+      <c r="O32" s="6">
+        <v>-0.8676593765172278</v>
+      </c>
+      <c r="P32" s="6">
+        <v>0.78249579446324091</v>
+      </c>
+      <c r="Q32" s="6">
+        <v>0.8879799220581378</v>
+      </c>
+      <c r="R32" s="6">
+        <v>-0.71244064669737173</v>
+      </c>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+      <c r="X32" s="6"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
+        <v>109</v>
+      </c>
+      <c r="B33">
         <v>21.4</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>4</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>121</v>
-      </c>
-      <c r="D33">
-        <v>109</v>
       </c>
       <c r="E33">
         <v>4.1100000000000003</v>
@@ -2052,6 +4042,1291 @@
       </c>
       <c r="K33">
         <v>2</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N33" s="6">
+        <v>-0.70822338886195324</v>
+      </c>
+      <c r="O33" s="6">
+        <v>0.41868403392177822</v>
+      </c>
+      <c r="P33" s="6">
+        <v>-0.59124207376886861</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>-0.4336978808110139</v>
+      </c>
+      <c r="R33" s="6">
+        <v>9.1204759651182993E-2</v>
+      </c>
+      <c r="S33" s="6">
+        <v>-0.17471587871340488</v>
+      </c>
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+      <c r="X33" s="6"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N34" s="6">
+        <v>-0.72309673735244961</v>
+      </c>
+      <c r="O34" s="6">
+        <v>0.66403891912759294</v>
+      </c>
+      <c r="P34" s="6">
+        <v>-0.81081179608300535</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>-0.71041589079060019</v>
+      </c>
+      <c r="R34" s="6">
+        <v>0.44027846495534917</v>
+      </c>
+      <c r="S34" s="6">
+        <v>-0.55491567766399397</v>
+      </c>
+      <c r="T34" s="6">
+        <v>0.74453544352625423</v>
+      </c>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+      <c r="X34" s="6"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="6">
+        <v>-0.24320425718585106</v>
+      </c>
+      <c r="O35" s="6">
+        <v>0.59983242945464765</v>
+      </c>
+      <c r="P35" s="6">
+        <v>-0.52260704690067539</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>-0.59122704006394744</v>
+      </c>
+      <c r="R35" s="6">
+        <v>0.71271112722626973</v>
+      </c>
+      <c r="S35" s="6">
+        <v>-0.69249525883948415</v>
+      </c>
+      <c r="T35" s="6">
+        <v>-0.22986086218488297</v>
+      </c>
+      <c r="U35" s="6">
+        <v>0.16834512458535861</v>
+      </c>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="M36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" s="6">
+        <v>-0.12570425822547418</v>
+      </c>
+      <c r="O36" s="6">
+        <v>0.48028475733884218</v>
+      </c>
+      <c r="P36" s="6">
+        <v>-0.49268659938947124</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>-0.55556919856248266</v>
+      </c>
+      <c r="R36" s="6">
+        <v>0.6996101319346647</v>
+      </c>
+      <c r="S36" s="6">
+        <v>-0.58328699653664795</v>
+      </c>
+      <c r="T36" s="6">
+        <v>-0.21268222972036493</v>
+      </c>
+      <c r="U36" s="6">
+        <v>0.20602334873357925</v>
+      </c>
+      <c r="V36" s="6">
+        <v>0.79405876025634348</v>
+      </c>
+      <c r="W36" s="6"/>
+      <c r="X36" s="6"/>
+    </row>
+    <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" s="7">
+        <v>0.74981247154911024</v>
+      </c>
+      <c r="O37" s="7">
+        <v>-0.55092507390245871</v>
+      </c>
+      <c r="P37" s="7">
+        <v>0.52698829374964329</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0.39497686486896932</v>
+      </c>
+      <c r="R37" s="7">
+        <v>-9.0789798868867275E-2</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0.42760593773548722</v>
+      </c>
+      <c r="T37" s="7">
+        <v>-0.65624922833805888</v>
+      </c>
+      <c r="U37" s="7">
+        <v>-0.56960714100684262</v>
+      </c>
+      <c r="V37" s="7">
+        <v>5.7534351070504114E-2</v>
+      </c>
+      <c r="W37" s="7">
+        <v>0.27407283635752228</v>
+      </c>
+      <c r="X37" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AF17:AI17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="N28:X37">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D6DA72-B58B-480C-95E6-371AD27C0C86}">
+  <dimension ref="A1:O37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>2.62</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+      <c r="E2" s="13">
+        <f>$H$26+($H$27*A2)+($H$28*B2)+($H$29*C2)</f>
+        <v>24.422057814190499</v>
+      </c>
+      <c r="F2" s="13">
+        <f>D2-E2</f>
+        <v>-3.4220578141904987</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>2.875</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E33" si="0">$H$26+($H$27*A3)+($H$28*B3)+($H$29*C3)</f>
+        <v>23.688021083669668</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" ref="F3:F37" si="1">D3-E3</f>
+        <v>-2.6880210836696676</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>93</v>
+      </c>
+      <c r="B4">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>22.8</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>25.922768779540149</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="1"/>
+        <v>-3.1227687795401486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>3.2149999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>21.4</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>20.625595312651924</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="1"/>
+        <v>0.77440468734807411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>175</v>
+      </c>
+      <c r="B6">
+        <v>3.44</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>18.7</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>17.54179865757547</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1582013424245297</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7">
+        <v>3.46</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>20.107737966036076</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="1"/>
+        <v>-2.0077379660360748</v>
+      </c>
+      <c r="G7" s="27" cm="1">
+        <f t="array" ref="G7:J7">LINEST(D2:D33,A2:C33)</f>
+        <v>2.0837101303232957</v>
+      </c>
+      <c r="H7" s="27">
+        <v>-2.8785754138071864</v>
+      </c>
+      <c r="I7" s="27">
+        <v>-3.7478725953382114E-2</v>
+      </c>
+      <c r="J7" s="27">
+        <v>34.002875122914062</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>245</v>
+      </c>
+      <c r="B8">
+        <v>3.57</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>14.3</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>14.544073037043789</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.24407303704378869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>3.19</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>24.4</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>22.496538543759449</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="1"/>
+        <v>1.9034614562405494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>95</v>
+      </c>
+      <c r="B10">
+        <v>3.15</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>22.8</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="0"/>
+        <v>21.374883603850126</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="1"/>
+        <v>1.4251163961498747</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>123</v>
+      </c>
+      <c r="B11">
+        <v>3.44</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>19.2</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="0"/>
+        <v>19.490692407151343</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.2906924071513437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>123</v>
+      </c>
+      <c r="B12">
+        <v>3.44</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>17.8</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>19.490692407151343</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.6906924071513423</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>4.07</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="0"/>
+        <v>15.540902517110032</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="1"/>
+        <v>0.85909748288996646</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="34">
+        <v>0.91645529354564448</v>
+      </c>
+      <c r="K13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="36">
+        <f>CORREL(D2:D33,E2:E33)</f>
+        <v>0.91645529354564448</v>
+      </c>
+      <c r="N13" s="16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(M13)</f>
+        <v>=CORREL(D2:D33,E2:E33)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>180</v>
+      </c>
+      <c r="B14">
+        <v>3.73</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>17.3</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="0"/>
+        <v>16.519618157804477</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="1"/>
+        <v>0.7803818421955242</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="35">
+        <v>0.83989030506783335</v>
+      </c>
+      <c r="K14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="37">
+        <f>M13^2</f>
+        <v>0.83989030506783335</v>
+      </c>
+      <c r="N14" s="16" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(M14)</f>
+        <v>=M13^2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>180</v>
+      </c>
+      <c r="B15">
+        <v>3.78</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>15.2</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="0"/>
+        <v>16.375689387114118</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.1756893871141187</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.82273569489652976</v>
+      </c>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>205</v>
+      </c>
+      <c r="B16">
+        <v>5.25</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>10.4</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="0"/>
+        <v>11.207215379983001</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.80721537998300086</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2.5375119399426995</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>215</v>
+      </c>
+      <c r="B17">
+        <v>5.4240000000000004</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>10.4</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="0"/>
+        <v>10.331555998446728</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="1"/>
+        <v>6.8444001553272571E-2</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>230</v>
+      </c>
+      <c r="B18">
+        <v>5.3449999999999998</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>14.7</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9967825668367674</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="1"/>
+        <v>4.7032174331632319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>32.4</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="0"/>
+        <v>27.280123429938328</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="1"/>
+        <v>5.1198765700616704</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>1.615</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>30.4</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="0"/>
+        <v>29.488792210362881</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="1"/>
+        <v>0.91120778963711757</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>65</v>
+      </c>
+      <c r="B21">
+        <v>1.835</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>33.9</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="0"/>
+        <v>28.368282181931335</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="1"/>
+        <v>5.5317178180686639</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1">
+        <v>945.75611583015075</v>
+      </c>
+      <c r="J21" s="1">
+        <v>315.25203861005025</v>
+      </c>
+      <c r="K21" s="1">
+        <v>48.960034456091059</v>
+      </c>
+      <c r="L21" s="29">
+        <v>2.9078715492971068E-11</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>97</v>
+      </c>
+      <c r="B22">
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>21.5</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="0"/>
+        <v>23.271750310401284</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.7717503104012842</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1">
+        <v>180.29107166984934</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6.4389668453517626</v>
+      </c>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>150</v>
+      </c>
+      <c r="B23">
+        <v>3.52</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>15.5</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="0"/>
+        <v>18.248480773305452</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="1"/>
+        <v>-2.7484807733054524</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="2">
+        <v>31</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1126.0471875000001</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>150</v>
+      </c>
+      <c r="B24">
+        <v>3.4350000000000001</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>15.2</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="0"/>
+        <v>18.49315968347906</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="1"/>
+        <v>-3.2931596834790611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>245</v>
+      </c>
+      <c r="B25">
+        <v>3.84</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>13.3</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="0"/>
+        <v>13.766857675315849</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.46685767531584865</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>175</v>
+      </c>
+      <c r="B26">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>19.2</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="0"/>
+        <v>16.37597561498356</v>
+      </c>
+      <c r="F26" s="13">
+        <f t="shared" si="1"/>
+        <v>2.8240243850164397</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="1">
+        <v>34.002875122914062</v>
+      </c>
+      <c r="I26" s="1">
+        <v>2.6426593369900306</v>
+      </c>
+      <c r="J26" s="1">
+        <v>12.866915779482603</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2.8240301965831147E-13</v>
+      </c>
+      <c r="L26" s="1">
+        <v>28.589632863691797</v>
+      </c>
+      <c r="M26" s="1">
+        <v>39.416117382136328</v>
+      </c>
+      <c r="N26" s="1">
+        <v>28.589632863691797</v>
+      </c>
+      <c r="O26" s="1">
+        <v>39.416117382136328</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>66</v>
+      </c>
+      <c r="B27">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>27.3</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="0"/>
+        <v>28.042945914597233</v>
+      </c>
+      <c r="F27" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.74294591459723236</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="28">
+        <v>-3.7478725953382114E-2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>9.6054221574033462E-3</v>
+      </c>
+      <c r="J27" s="1">
+        <v>-3.90183016833836</v>
+      </c>
+      <c r="K27" s="32">
+        <v>5.4640226580877677E-4</v>
+      </c>
+      <c r="L27" s="1">
+        <v>-5.7154541300565409E-2</v>
+      </c>
+      <c r="M27" s="1">
+        <v>-1.7802910606198815E-2</v>
+      </c>
+      <c r="N27" s="1">
+        <v>-5.7154541300565409E-2</v>
+      </c>
+      <c r="O27" s="1">
+        <v>-1.7802910606198815E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>2.14</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="0"/>
+        <v>26.515869805932208</v>
+      </c>
+      <c r="F28" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.51586980593220844</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="28">
+        <v>-2.8785754138071864</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.90497053803057714</v>
+      </c>
+      <c r="J28" s="1">
+        <v>-3.1808498650924313</v>
+      </c>
+      <c r="K28" s="32">
+        <v>3.5740310794737246E-3</v>
+      </c>
+      <c r="L28" s="1">
+        <v>-4.7323235270233059</v>
+      </c>
+      <c r="M28" s="1">
+        <v>-1.0248273005910673</v>
+      </c>
+      <c r="N28" s="1">
+        <v>-4.7323235270233059</v>
+      </c>
+      <c r="O28" s="1">
+        <v>-1.0248273005910673</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>113</v>
+      </c>
+      <c r="B29">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>30.4</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>27.496204619414907</v>
+      </c>
+      <c r="F29" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9037953805850911</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="23">
+        <v>2.0837101303232957</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1.3764201523049431</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.5138619750909124</v>
+      </c>
+      <c r="K29" s="33">
+        <v>0.14126823673653088</v>
+      </c>
+      <c r="L29" s="2">
+        <v>-0.73575873976904793</v>
+      </c>
+      <c r="M29" s="2">
+        <v>4.9031790004156388</v>
+      </c>
+      <c r="N29" s="2">
+        <v>-0.73575873976904793</v>
+      </c>
+      <c r="O29" s="2">
+        <v>4.9031790004156388</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>264</v>
+      </c>
+      <c r="B30">
+        <v>3.17</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>15.8</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>17.067117539775701</v>
+      </c>
+      <c r="F30" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.2671175397757004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>175</v>
+      </c>
+      <c r="B31">
+        <v>2.77</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>19.7</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>21.554154315149582</v>
+      </c>
+      <c r="F31" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.8541543151495823</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>335</v>
+      </c>
+      <c r="B32">
+        <v>3.57</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>13.254697831562694</v>
+      </c>
+      <c r="F32" s="13">
+        <f t="shared" si="1"/>
+        <v>1.7453021684373056</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>109</v>
+      </c>
+      <c r="B33">
+        <v>2.78</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>21.4</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>23.998964473934734</v>
+      </c>
+      <c r="F33" s="13">
+        <f t="shared" si="1"/>
+        <v>-2.5989644739347355</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F34" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>200</v>
+      </c>
+      <c r="J34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F35" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <v>3.5</v>
+      </c>
+      <c r="J35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F36" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F37" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="31">
+        <f>H26+(H27*H34)+(H35*H28)+(H29*H36)</f>
+        <v>18.515826114235786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized mtcars Statistics with Excel - Sum squared error - RMSE
</commit_message>
<xml_diff>
--- a/Intro to Statistics/mtcars.xlsx
+++ b/Intro to Statistics/mtcars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Online Learning\DataRockie Bootcamp\DataRockie Bootcamp 10th\Intro to Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3F4F95-6259-4328-BCFA-66DDA9FD8F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF95BE7B-62D4-4AD2-B23D-39131373AFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="66">
   <si>
     <t>mpg</t>
   </si>
@@ -251,6 +251,18 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>error^2</t>
+  </si>
+  <si>
+    <t>Sum squared error</t>
+  </si>
+  <si>
+    <t>Minimize</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
@@ -258,8 +270,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -616,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -751,6 +763,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -796,58 +817,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2523,12 +2541,12 @@
       <c r="K2">
         <v>4</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <f>CORREL(B2:B33,A2:A33)</f>
         <v>-0.77616837182658638</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
       <c r="U2" t="s">
         <v>12</v>
       </c>
@@ -2567,9 +2585,9 @@
       <c r="K3">
         <v>4</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
       <c r="U3" t="s">
         <v>13</v>
       </c>
@@ -2611,11 +2629,11 @@
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10" t="s">
+      <c r="M4" s="8"/>
+      <c r="N4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="8" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2653,28 +2671,28 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="15">
+      <c r="N5" s="12">
         <v>1</v>
       </c>
-      <c r="O5" s="4"/>
+      <c r="O5" s="3"/>
       <c r="U5" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="17">
+      <c r="V5" s="14">
         <f>INTERCEPT($B$2:$B$33,$A$2:$A$33)</f>
         <v>30.098860539622493</v>
       </c>
-      <c r="W5" s="16" t="str">
+      <c r="W5" s="13" t="str">
         <f ca="1">_xlfn.FORMULATEXT(V5)</f>
         <v>=INTERCEPT($B$2:$B$33,$A$2:$A$33)</v>
       </c>
-      <c r="AA5" s="18" t="s">
+      <c r="AA5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AB5" s="18"/>
+      <c r="AB5" s="15"/>
     </row>
     <row r="6" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -2710,36 +2728,36 @@
       <c r="K6">
         <v>2</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11">
+      <c r="M6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="9">
         <v>-0.77616837182658638</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="11">
         <v>1</v>
       </c>
       <c r="U6" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="17">
+      <c r="V6" s="14">
         <f>SLOPE($B$2:$B$33,$A$2:$A$33)</f>
         <v>-6.8228278071563661E-2</v>
       </c>
-      <c r="W6" s="16" t="str">
+      <c r="W6" s="13" t="str">
         <f ca="1">_xlfn.FORMULATEXT(V6)</f>
         <v>=SLOPE($B$2:$B$33,$A$2:$A$33)</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" t="s">
         <v>18</v>
       </c>
-      <c r="AB6" s="6">
+      <c r="AB6" s="5">
         <v>0.77616837182658638</v>
       </c>
       <c r="AD6" t="s">
         <v>39</v>
       </c>
-      <c r="AE6" s="12">
+      <c r="AE6" s="5">
         <f>CORREL(B2:B33,A2:A33)</f>
         <v>-0.77616837182658638</v>
       </c>
@@ -2778,16 +2796,16 @@
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" t="s">
         <v>19</v>
       </c>
-      <c r="AB7" s="19">
+      <c r="AB7" s="16">
         <v>0.60243734142393413</v>
       </c>
       <c r="AD7" t="s">
         <v>40</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AE7" s="5">
         <f>AE6^2</f>
         <v>0.60243734142393401</v>
       </c>
@@ -2829,10 +2847,10 @@
       <c r="K8">
         <v>4</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA8" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="AB8" s="5">
         <v>0.589185252804732</v>
       </c>
     </row>
@@ -2870,10 +2888,10 @@
       <c r="K9">
         <v>2</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AA9" t="s">
         <v>21</v>
       </c>
-      <c r="AB9" s="6">
+      <c r="AB9" s="5">
         <v>3.8629622206479564</v>
       </c>
     </row>
@@ -2911,10 +2929,10 @@
       <c r="K10">
         <v>2</v>
       </c>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AB10" s="1">
         <v>32</v>
       </c>
     </row>
@@ -2990,7 +3008,7 @@
       <c r="AA12" t="s">
         <v>23</v>
       </c>
-      <c r="AB12" s="16" t="s">
+      <c r="AB12" s="13" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3028,20 +3046,20 @@
       <c r="K13">
         <v>3</v>
       </c>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3" t="s">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC13" s="3" t="s">
+      <c r="AC13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD13" s="3" t="s">
+      <c r="AD13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE13" s="3" t="s">
+      <c r="AE13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF13" s="3" t="s">
+      <c r="AF13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3079,28 +3097,28 @@
       <c r="K14">
         <v>3</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AA14" t="s">
         <v>24</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AB14">
         <v>1</v>
       </c>
-      <c r="AC14" s="6">
+      <c r="AC14" s="5">
         <v>678.37287395539829</v>
       </c>
-      <c r="AD14" s="6">
+      <c r="AD14" s="5">
         <v>678.37287395539829</v>
       </c>
-      <c r="AE14" s="6">
+      <c r="AE14" s="5">
         <v>45.459803260823819</v>
       </c>
-      <c r="AF14" s="20">
+      <c r="AF14" s="17">
         <v>1.7878352541210598E-7</v>
       </c>
-      <c r="AG14" s="16" t="s">
+      <c r="AG14" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AH14" s="22" t="s">
+      <c r="AH14" s="19" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3138,20 +3156,20 @@
       <c r="K15">
         <v>3</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AA15" t="s">
         <v>25</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AB15">
         <v>30</v>
       </c>
-      <c r="AC15" s="6">
+      <c r="AC15" s="5">
         <v>447.67431354460172</v>
       </c>
-      <c r="AD15" s="6">
+      <c r="AD15" s="5">
         <v>14.92247711815339</v>
       </c>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
     </row>
     <row r="16" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -3187,18 +3205,18 @@
       <c r="K16">
         <v>4</v>
       </c>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AB16" s="1">
         <v>31</v>
       </c>
-      <c r="AC16" s="7">
+      <c r="AC16" s="6">
         <v>1126.0471875000001</v>
       </c>
-      <c r="AD16" s="7"/>
-      <c r="AE16" s="7"/>
-      <c r="AF16" s="7"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
     </row>
     <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
@@ -3234,12 +3252,12 @@
       <c r="K17">
         <v>4</v>
       </c>
-      <c r="AF17" s="26" t="s">
+      <c r="AF17" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="AG17" s="26"/>
-      <c r="AH17" s="26"/>
-      <c r="AI17" s="26"/>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="31"/>
+      <c r="AI17" s="31"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18">
@@ -3275,29 +3293,29 @@
       <c r="K18">
         <v>4</v>
       </c>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3" t="s">
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AC18" s="3" t="s">
+      <c r="AC18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AD18" s="3" t="s">
+      <c r="AD18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AE18" s="3" t="s">
+      <c r="AE18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AF18" s="3" t="s">
+      <c r="AF18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AG18" s="3" t="s">
+      <c r="AG18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AH18" s="3" t="s">
+      <c r="AH18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AI18" s="3" t="s">
+      <c r="AI18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3335,31 +3353,31 @@
       <c r="K19">
         <v>1</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AA19" t="s">
         <v>14</v>
       </c>
-      <c r="AB19" s="20">
+      <c r="AB19" s="17">
         <v>30.098860539622493</v>
       </c>
-      <c r="AC19" s="6">
+      <c r="AC19" s="5">
         <v>1.633920950302906</v>
       </c>
-      <c r="AD19" s="6">
+      <c r="AD19" s="5">
         <v>18.421246470976815</v>
       </c>
-      <c r="AE19" s="20">
+      <c r="AE19" s="17">
         <v>6.6427360304650858E-18</v>
       </c>
-      <c r="AF19" s="6">
+      <c r="AF19" s="5">
         <v>26.761948787045323</v>
       </c>
-      <c r="AG19" s="6">
+      <c r="AG19" s="5">
         <v>33.435772292199658</v>
       </c>
-      <c r="AH19" s="6">
+      <c r="AH19" s="5">
         <v>26.761948787045323</v>
       </c>
-      <c r="AI19" s="6">
+      <c r="AI19" s="5">
         <v>33.435772292199658</v>
       </c>
     </row>
@@ -3397,31 +3415,31 @@
       <c r="K20">
         <v>2</v>
       </c>
-      <c r="AA20" s="24" t="s">
+      <c r="AA20" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="AB20" s="21">
+      <c r="AB20" s="18">
         <v>-6.8228278071563689E-2</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="AC20" s="6">
         <v>1.0119303810422772E-2</v>
       </c>
-      <c r="AD20" s="7">
+      <c r="AD20" s="6">
         <v>-6.7423885427067924</v>
       </c>
-      <c r="AE20" s="21">
+      <c r="AE20" s="18">
         <v>1.7878352541210566E-7</v>
       </c>
-      <c r="AF20" s="21">
+      <c r="AF20" s="18">
         <v>-8.8894653520534272E-2</v>
       </c>
-      <c r="AG20" s="21">
+      <c r="AG20" s="18">
         <v>-4.7561902622593098E-2</v>
       </c>
-      <c r="AH20" s="21">
+      <c r="AH20" s="18">
         <v>-8.8894653520534272E-2</v>
       </c>
-      <c r="AI20" s="21">
+      <c r="AI20" s="18">
         <v>-4.7561902622593098E-2</v>
       </c>
     </row>
@@ -3605,14 +3623,14 @@
       <c r="K25">
         <v>4</v>
       </c>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AA25" s="25">
+      <c r="AA25" s="22">
         <f>AB19+(AB20*200)</f>
         <v>16.453204925309755</v>
       </c>
-      <c r="AB25" s="16" t="s">
+      <c r="AB25" s="13" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3650,38 +3668,38 @@
       <c r="K26">
         <v>2</v>
       </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3" t="s">
+      <c r="M26" s="2"/>
+      <c r="N26" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P26" s="3" t="s">
+      <c r="O26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="Q26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="R26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S26" s="3" t="s">
+      <c r="S26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="T26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U26" s="3" t="s">
+      <c r="U26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V26" s="3" t="s">
+      <c r="V26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="W26" s="3" t="s">
+      <c r="W26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X26" s="3" t="s">
+      <c r="X26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3719,20 +3737,20 @@
       <c r="K27">
         <v>1</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M27" t="s">
         <v>3</v>
       </c>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
-      <c r="T27" s="6"/>
-      <c r="U27" s="6"/>
-      <c r="V27" s="6"/>
-      <c r="W27" s="6"/>
-      <c r="X27" s="6"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -3768,22 +3786,22 @@
       <c r="K28">
         <v>2</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6">
+      <c r="M28" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" s="5">
         <v>-0.77616837182658638</v>
       </c>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6"/>
-      <c r="U28" s="6"/>
-      <c r="V28" s="6"/>
-      <c r="W28" s="6"/>
-      <c r="X28" s="6"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -3819,24 +3837,24 @@
       <c r="K29">
         <v>2</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="M29" t="s">
         <v>1</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29" s="5">
         <v>0.83244745272181953</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="5">
         <v>-0.8521619594266131</v>
       </c>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -3872,26 +3890,26 @@
       <c r="K30">
         <v>4</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="M30" t="s">
         <v>2</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="5">
         <v>0.79094858636980647</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="5">
         <v>-0.84755137926247848</v>
       </c>
-      <c r="P30" s="6">
+      <c r="P30" s="5">
         <v>0.9020328721469989</v>
       </c>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -3927,28 +3945,28 @@
       <c r="K31">
         <v>6</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="M31" t="s">
         <v>4</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31" s="5">
         <v>-0.44875911687291947</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="5">
         <v>0.68117190780674908</v>
       </c>
-      <c r="P31" s="6">
+      <c r="P31" s="5">
         <v>-0.69993811382876991</v>
       </c>
-      <c r="Q31" s="6">
+      <c r="Q31" s="5">
         <v>-0.71021392716927001</v>
       </c>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
-      <c r="T31" s="6"/>
-      <c r="U31" s="6"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -3984,30 +4002,30 @@
       <c r="K32">
         <v>8</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="M32" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32" s="5">
         <v>0.6587478873447592</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="5">
         <v>-0.8676593765172278</v>
       </c>
-      <c r="P32" s="6">
+      <c r="P32" s="5">
         <v>0.78249579446324091</v>
       </c>
-      <c r="Q32" s="6">
+      <c r="Q32" s="5">
         <v>0.8879799220581378</v>
       </c>
-      <c r="R32" s="6">
+      <c r="R32" s="5">
         <v>-0.71244064669737173</v>
       </c>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
@@ -4043,164 +4061,164 @@
       <c r="K33">
         <v>2</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="M33" t="s">
         <v>6</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="5">
         <v>-0.70822338886195324</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="5">
         <v>0.41868403392177822</v>
       </c>
-      <c r="P33" s="6">
+      <c r="P33" s="5">
         <v>-0.59124207376886861</v>
       </c>
-      <c r="Q33" s="6">
+      <c r="Q33" s="5">
         <v>-0.4336978808110139</v>
       </c>
-      <c r="R33" s="6">
+      <c r="R33" s="5">
         <v>9.1204759651182993E-2</v>
       </c>
-      <c r="S33" s="6">
+      <c r="S33" s="5">
         <v>-0.17471587871340488</v>
       </c>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M34" s="1" t="s">
+      <c r="M34" t="s">
         <v>7</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="5">
         <v>-0.72309673735244961</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
         <v>0.66403891912759294</v>
       </c>
-      <c r="P34" s="6">
+      <c r="P34" s="5">
         <v>-0.81081179608300535</v>
       </c>
-      <c r="Q34" s="6">
+      <c r="Q34" s="5">
         <v>-0.71041589079060019</v>
       </c>
-      <c r="R34" s="6">
+      <c r="R34" s="5">
         <v>0.44027846495534917</v>
       </c>
-      <c r="S34" s="6">
+      <c r="S34" s="5">
         <v>-0.55491567766399397</v>
       </c>
-      <c r="T34" s="6">
+      <c r="T34" s="5">
         <v>0.74453544352625423</v>
       </c>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M35" s="1" t="s">
+      <c r="M35" t="s">
         <v>8</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="5">
         <v>-0.24320425718585106</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="5">
         <v>0.59983242945464765</v>
       </c>
-      <c r="P35" s="6">
+      <c r="P35" s="5">
         <v>-0.52260704690067539</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q35" s="5">
         <v>-0.59122704006394744</v>
       </c>
-      <c r="R35" s="6">
+      <c r="R35" s="5">
         <v>0.71271112722626973</v>
       </c>
-      <c r="S35" s="6">
+      <c r="S35" s="5">
         <v>-0.69249525883948415</v>
       </c>
-      <c r="T35" s="6">
+      <c r="T35" s="5">
         <v>-0.22986086218488297</v>
       </c>
-      <c r="U35" s="6">
+      <c r="U35" s="5">
         <v>0.16834512458535861</v>
       </c>
-      <c r="V35" s="6"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="6"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
+      <c r="X35" s="5"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M36" s="1" t="s">
+      <c r="M36" t="s">
         <v>9</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="5">
         <v>-0.12570425822547418</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
         <v>0.48028475733884218</v>
       </c>
-      <c r="P36" s="6">
+      <c r="P36" s="5">
         <v>-0.49268659938947124</v>
       </c>
-      <c r="Q36" s="6">
+      <c r="Q36" s="5">
         <v>-0.55556919856248266</v>
       </c>
-      <c r="R36" s="6">
+      <c r="R36" s="5">
         <v>0.6996101319346647</v>
       </c>
-      <c r="S36" s="6">
+      <c r="S36" s="5">
         <v>-0.58328699653664795</v>
       </c>
-      <c r="T36" s="6">
+      <c r="T36" s="5">
         <v>-0.21268222972036493</v>
       </c>
-      <c r="U36" s="6">
+      <c r="U36" s="5">
         <v>0.20602334873357925</v>
       </c>
-      <c r="V36" s="6">
+      <c r="V36" s="5">
         <v>0.79405876025634348</v>
       </c>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
     </row>
     <row r="37" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M37" s="2" t="s">
+      <c r="M37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N37" s="7">
+      <c r="N37" s="6">
         <v>0.74981247154911024</v>
       </c>
-      <c r="O37" s="7">
+      <c r="O37" s="6">
         <v>-0.55092507390245871</v>
       </c>
-      <c r="P37" s="7">
+      <c r="P37" s="6">
         <v>0.52698829374964329</v>
       </c>
-      <c r="Q37" s="7">
+      <c r="Q37" s="6">
         <v>0.39497686486896932</v>
       </c>
-      <c r="R37" s="7">
+      <c r="R37" s="6">
         <v>-9.0789798868867275E-2</v>
       </c>
-      <c r="S37" s="7">
+      <c r="S37" s="6">
         <v>0.42760593773548722</v>
       </c>
-      <c r="T37" s="7">
+      <c r="T37" s="6">
         <v>-0.65624922833805888</v>
       </c>
-      <c r="U37" s="7">
+      <c r="U37" s="6">
         <v>-0.56960714100684262</v>
       </c>
-      <c r="V37" s="7">
+      <c r="V37" s="6">
         <v>5.7534351070504114E-2</v>
       </c>
-      <c r="W37" s="7">
+      <c r="W37" s="6">
         <v>0.27407283635752228</v>
       </c>
-      <c r="X37" s="7"/>
+      <c r="X37" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4218,25 +4236,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D6DA72-B58B-480C-95E6-371AD27C0C86}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" customWidth="1"/>
+    <col min="5" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
+    <col min="10" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
+    <col min="15" max="15" width="12.77734375" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" customWidth="1"/>
+    <col min="20" max="20" width="10.88671875" customWidth="1"/>
+    <col min="21" max="21" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4252,11 +4273,19 @@
       <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="30" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G1" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>110</v>
       </c>
@@ -4269,19 +4298,30 @@
       <c r="D2">
         <v>21</v>
       </c>
-      <c r="E2" s="13">
-        <f>$H$26+($H$27*A2)+($H$28*B2)+($H$29*C2)</f>
+      <c r="E2" s="10">
+        <f>$N$26+($N$27*A2)+($N$28*B2)+($N$29*C2)</f>
         <v>24.422057814190499</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="10">
         <f>D2-E2</f>
         <v>-3.4220578141904987</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10">
+        <f t="array" ref="G2:G33">F2:F33^2</f>
+        <v>11.710479683662253</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>110</v>
       </c>
@@ -4294,19 +4334,32 @@
       <c r="D3">
         <v>21</v>
       </c>
-      <c r="E3" s="13">
-        <f t="shared" ref="E3:E33" si="0">$H$26+($H$27*A3)+($H$28*B3)+($H$29*C3)</f>
+      <c r="E3" s="10">
+        <f t="shared" ref="E3:E33" si="0">$N$26+($N$27*A3)+($N$28*B3)+($N$29*C3)</f>
         <v>23.688021083669668</v>
       </c>
-      <c r="F3" s="13">
-        <f t="shared" ref="F3:F37" si="1">D3-E3</f>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F33" si="1">D3-E3</f>
         <v>-2.6880210836696676</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="10">
+        <v>7.2254573462526546</v>
+      </c>
+      <c r="H3" s="10"/>
+      <c r="I3" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="10">
+        <f>SUM(G2:G33)</f>
+        <v>180.2910716698494</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>93</v>
       </c>
@@ -4319,16 +4372,24 @@
       <c r="D4">
         <v>22.8</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <f t="shared" si="0"/>
         <v>25.922768779540149</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="10">
         <f t="shared" si="1"/>
         <v>-3.1227687795401486</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G4" s="10">
+        <v>9.751684850470669</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>110</v>
       </c>
@@ -4341,16 +4402,29 @@
       <c r="D5">
         <v>21.4</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>20.625595312651924</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="10">
         <f t="shared" si="1"/>
         <v>0.77440468734807411</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G5" s="10">
+        <v>0.59970261978666839</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="10">
+        <f>SQRT(AVERAGE(G2:G33))</f>
+        <v>2.3736250735284194</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>175</v>
       </c>
@@ -4363,28 +4437,36 @@
       <c r="D6">
         <v>18.7</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>17.54179865757547</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="10">
         <f t="shared" si="1"/>
         <v>1.1582013424245297</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10">
+        <v>1.3414303495939826</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" t="s">
         <v>8</v>
       </c>
-      <c r="H6" t="s">
+      <c r="N6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6" t="s">
         <v>3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="P6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105</v>
       </c>
@@ -4397,29 +4479,37 @@
       <c r="D7">
         <v>18.100000000000001</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <f t="shared" si="0"/>
         <v>20.107737966036076</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="10">
         <f t="shared" si="1"/>
         <v>-2.0077379660360748</v>
       </c>
-      <c r="G7" s="27" cm="1">
-        <f t="array" ref="G7:J7">LINEST(D2:D33,A2:C33)</f>
+      <c r="G7" s="10">
+        <v>4.0310117402626746</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="23" cm="1">
+        <f t="array" ref="M7:P7">LINEST(D2:D33,A2:C33)</f>
         <v>2.0837101303232957</v>
       </c>
-      <c r="H7" s="27">
+      <c r="N7" s="23">
         <v>-2.8785754138071864</v>
       </c>
-      <c r="I7" s="27">
+      <c r="O7" s="23">
         <v>-3.7478725953382114E-2</v>
       </c>
-      <c r="J7" s="27">
+      <c r="P7" s="23">
         <v>34.002875122914062</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>245</v>
       </c>
@@ -4432,16 +4522,24 @@
       <c r="D8">
         <v>14.3</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>14.544073037043789</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="10">
         <f t="shared" si="1"/>
         <v>-0.24407303704378869</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G8" s="10">
+        <v>5.9571647411778644E-2</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>62</v>
       </c>
@@ -4454,16 +4552,24 @@
       <c r="D9">
         <v>24.4</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <f t="shared" si="0"/>
         <v>22.496538543759449</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="10">
         <f t="shared" si="1"/>
         <v>1.9034614562405494</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G9" s="10">
+        <v>3.623165515393393</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>95</v>
       </c>
@@ -4476,19 +4582,27 @@
       <c r="D10">
         <v>22.8</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>21.374883603850126</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="10">
         <f t="shared" si="1"/>
         <v>1.4251163961498747</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10">
+        <v>2.0309567425752069</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>123</v>
       </c>
@@ -4501,16 +4615,24 @@
       <c r="D11">
         <v>19.2</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
         <v>19.490692407151343</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="10">
         <f t="shared" si="1"/>
         <v>-0.2906924071513437</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G11" s="10">
+        <v>8.4502075575442578E-2</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>123</v>
       </c>
@@ -4523,26 +4645,34 @@
       <c r="D12">
         <v>17.8</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
         <v>19.490692407151343</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="10">
         <f t="shared" si="1"/>
         <v>-1.6906924071513423</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="10">
+        <v>2.8584408155992</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="K12" t="s">
+      <c r="N12" s="15"/>
+      <c r="Q12" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="38" t="s">
+      <c r="S12" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>180</v>
       </c>
@@ -4555,33 +4685,41 @@
       <c r="D13">
         <v>16.399999999999999</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <f t="shared" si="0"/>
         <v>15.540902517110032</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <f t="shared" si="1"/>
         <v>0.85909748288996646</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="10">
+        <v>0.73804848510787624</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="34">
+      <c r="N13" s="28">
         <v>0.91645529354564448</v>
       </c>
-      <c r="K13" t="s">
+      <c r="Q13" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="36">
+      <c r="S13" s="28">
         <f>CORREL(D2:D33,E2:E33)</f>
         <v>0.91645529354564448</v>
       </c>
-      <c r="N13" s="16" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(M13)</f>
+      <c r="T13" s="13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(S13)</f>
         <v>=CORREL(D2:D33,E2:E33)</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>180</v>
       </c>
@@ -4594,33 +4732,41 @@
       <c r="D14">
         <v>17.3</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="10">
         <f t="shared" si="0"/>
         <v>16.519618157804477</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="10">
         <f t="shared" si="1"/>
         <v>0.7803818421955242</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="10">
+        <v>0.60899581962848004</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="35">
+      <c r="N14" s="29">
         <v>0.83989030506783335</v>
       </c>
-      <c r="K14" t="s">
+      <c r="Q14" t="s">
         <v>55</v>
       </c>
-      <c r="M14" s="37">
-        <f>M13^2</f>
+      <c r="S14" s="29">
+        <f>S13^2</f>
         <v>0.83989030506783335</v>
       </c>
-      <c r="N14" s="16" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(M14)</f>
-        <v>=M13^2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="T14" s="13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(S14)</f>
+        <v>=S13^2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>180</v>
       </c>
@@ -4633,23 +4779,31 @@
       <c r="D15">
         <v>15.2</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="10">
         <f t="shared" si="0"/>
         <v>16.375689387114118</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="10">
         <f t="shared" si="1"/>
         <v>-1.1756893871141187</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="10">
+        <v>1.3822455349727722</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="4">
+      <c r="N15" s="3">
         <v>0.82273569489652976</v>
       </c>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>205</v>
       </c>
@@ -4662,25 +4816,33 @@
       <c r="D16">
         <v>10.4</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="10">
         <f t="shared" si="0"/>
         <v>11.207215379983001</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="10">
         <f t="shared" si="1"/>
         <v>-0.80721537998300086</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="10">
+        <v>0.65159666968110042</v>
+      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="4">
+      <c r="N16" s="3">
         <v>2.5375119399426995</v>
       </c>
-      <c r="M16" s="16" t="s">
+      <c r="S16" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>215</v>
       </c>
@@ -4693,22 +4855,30 @@
       <c r="D17">
         <v>10.4</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="10">
         <f t="shared" si="0"/>
         <v>10.331555998446728</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="10">
         <f t="shared" si="1"/>
         <v>6.8444001553272571E-2</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="10">
+        <v>4.6845813486243778E-3</v>
+      </c>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="2">
+      <c r="N17" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>230</v>
       </c>
@@ -4721,16 +4891,24 @@
       <c r="D18">
         <v>14.7</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="10">
         <f t="shared" si="0"/>
         <v>9.9967825668367674</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="10">
         <f t="shared" si="1"/>
         <v>4.7032174331632319</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="10">
+        <v>22.120254223610541</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>66</v>
       </c>
@@ -4743,19 +4921,27 @@
       <c r="D19">
         <v>32.4</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <f t="shared" si="0"/>
         <v>27.280123429938328</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="10">
         <f t="shared" si="1"/>
         <v>5.1198765700616704</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="10">
+        <v>26.213136092666456</v>
+      </c>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>52</v>
       </c>
@@ -4768,32 +4954,40 @@
       <c r="D20">
         <v>30.4</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="10">
         <f t="shared" si="0"/>
         <v>29.488792210362881</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="10">
         <f t="shared" si="1"/>
         <v>0.91120778963711757</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="10">
+        <v>0.83029963589536149</v>
+      </c>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="O20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="P20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="Q20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="R20" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>65</v>
       </c>
@@ -4806,40 +5000,48 @@
       <c r="D21">
         <v>33.9</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="10">
         <f t="shared" si="0"/>
         <v>28.368282181931335</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="10">
         <f t="shared" si="1"/>
         <v>5.5317178180686639</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="10">
+        <v>30.599902018738341</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1">
+      <c r="N21">
         <v>3</v>
       </c>
-      <c r="I21" s="1">
+      <c r="O21">
         <v>945.75611583015075</v>
       </c>
-      <c r="J21" s="1">
+      <c r="P21">
         <v>315.25203861005025</v>
       </c>
-      <c r="K21" s="1">
+      <c r="Q21">
         <v>48.960034456091059</v>
       </c>
-      <c r="L21" s="29">
+      <c r="R21" s="24">
         <v>2.9078715492971068E-11</v>
       </c>
-      <c r="M21" s="16" t="s">
+      <c r="S21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="N21" s="16" t="s">
+      <c r="T21" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>97</v>
       </c>
@@ -4852,33 +5054,39 @@
       <c r="D22">
         <v>21.5</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="10">
         <f t="shared" si="0"/>
         <v>23.271750310401284</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="10">
         <f t="shared" si="1"/>
         <v>-1.7717503104012842</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="10">
+        <v>3.1390991624070468</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="1">
+      <c r="N22">
         <v>28</v>
       </c>
-      <c r="I22" s="1">
+      <c r="O22">
         <v>180.29107166984934</v>
       </c>
-      <c r="J22" s="1">
+      <c r="P22">
         <v>6.4389668453517626</v>
       </c>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" t="s">
+      <c r="S22" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>150</v>
       </c>
@@ -4891,28 +5099,36 @@
       <c r="D23">
         <v>15.5</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="10">
         <f t="shared" si="0"/>
         <v>18.248480773305452</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="10">
         <f t="shared" si="1"/>
         <v>-2.7484807733054524</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="10">
+        <v>7.5541465612297376</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="2">
+      <c r="N23" s="1">
         <v>31</v>
       </c>
-      <c r="I23" s="2">
+      <c r="O23" s="1">
         <v>1126.0471875000001</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>150</v>
       </c>
@@ -4925,16 +5141,24 @@
       <c r="D24">
         <v>15.2</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="10">
         <f t="shared" si="0"/>
         <v>18.49315968347906</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="10">
         <f t="shared" si="1"/>
         <v>-3.2931596834790611</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G24" s="10">
+        <v>10.844900700891909</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>245</v>
       </c>
@@ -4947,41 +5171,49 @@
       <c r="D25">
         <v>13.3</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="10">
         <f t="shared" si="0"/>
         <v>13.766857675315849</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="10">
         <f t="shared" si="1"/>
         <v>-0.46685767531584865</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="10">
+        <v>0.21795608900131835</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="O25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="P25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="Q25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="R25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="S25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="T25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="U25" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>175</v>
       </c>
@@ -4994,43 +5226,51 @@
       <c r="D26">
         <v>19.2</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="10">
         <f t="shared" si="0"/>
         <v>16.37597561498356</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="10">
         <f t="shared" si="1"/>
         <v>2.8240243850164397</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="10">
+        <v>7.9751137271674803</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="1">
+      <c r="N26">
         <v>34.002875122914062</v>
       </c>
-      <c r="I26" s="1">
+      <c r="O26">
         <v>2.6426593369900306</v>
       </c>
-      <c r="J26" s="1">
+      <c r="P26">
         <v>12.866915779482603</v>
       </c>
-      <c r="K26" s="1">
+      <c r="Q26">
         <v>2.8240301965831147E-13</v>
       </c>
-      <c r="L26" s="1">
+      <c r="R26">
         <v>28.589632863691797</v>
       </c>
-      <c r="M26" s="1">
+      <c r="S26">
         <v>39.416117382136328</v>
       </c>
-      <c r="N26" s="1">
+      <c r="T26">
         <v>28.589632863691797</v>
       </c>
-      <c r="O26" s="1">
+      <c r="U26">
         <v>39.416117382136328</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>66</v>
       </c>
@@ -5043,43 +5283,51 @@
       <c r="D27">
         <v>27.3</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="10">
         <f t="shared" si="0"/>
         <v>28.042945914597233</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="10">
         <f t="shared" si="1"/>
         <v>-0.74294591459723236</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="10">
+        <v>0.55196863201671809</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="28">
+      <c r="N27" s="23">
         <v>-3.7478725953382114E-2</v>
       </c>
-      <c r="I27" s="1">
+      <c r="O27">
         <v>9.6054221574033462E-3</v>
       </c>
-      <c r="J27" s="1">
+      <c r="P27">
         <v>-3.90183016833836</v>
       </c>
-      <c r="K27" s="32">
+      <c r="Q27" s="26">
         <v>5.4640226580877677E-4</v>
       </c>
-      <c r="L27" s="1">
+      <c r="R27">
         <v>-5.7154541300565409E-2</v>
       </c>
-      <c r="M27" s="1">
+      <c r="S27">
         <v>-1.7802910606198815E-2</v>
       </c>
-      <c r="N27" s="1">
+      <c r="T27">
         <v>-5.7154541300565409E-2</v>
       </c>
-      <c r="O27" s="1">
+      <c r="U27">
         <v>-1.7802910606198815E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>91</v>
       </c>
@@ -5092,43 +5340,51 @@
       <c r="D28">
         <v>26</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="10">
         <f t="shared" si="0"/>
         <v>26.515869805932208</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F28" s="10">
         <f t="shared" si="1"/>
         <v>-0.51586980593220844</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="10">
+        <v>0.2661216566725344</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="28">
+      <c r="N28" s="23">
         <v>-2.8785754138071864</v>
       </c>
-      <c r="I28" s="1">
+      <c r="O28">
         <v>0.90497053803057714</v>
       </c>
-      <c r="J28" s="1">
+      <c r="P28">
         <v>-3.1808498650924313</v>
       </c>
-      <c r="K28" s="32">
+      <c r="Q28" s="26">
         <v>3.5740310794737246E-3</v>
       </c>
-      <c r="L28" s="1">
+      <c r="R28">
         <v>-4.7323235270233059</v>
       </c>
-      <c r="M28" s="1">
+      <c r="S28">
         <v>-1.0248273005910673</v>
       </c>
-      <c r="N28" s="1">
+      <c r="T28">
         <v>-4.7323235270233059</v>
       </c>
-      <c r="O28" s="1">
+      <c r="U28">
         <v>-1.0248273005910673</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>113</v>
       </c>
@@ -5141,43 +5397,51 @@
       <c r="D29">
         <v>30.4</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="10">
         <f t="shared" si="0"/>
         <v>27.496204619414907</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F29" s="10">
         <f t="shared" si="1"/>
         <v>2.9037953805850911</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="10">
+        <v>8.4320276123073139</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="23">
+      <c r="N29" s="20">
         <v>2.0837101303232957</v>
       </c>
-      <c r="I29" s="2">
+      <c r="O29" s="1">
         <v>1.3764201523049431</v>
       </c>
-      <c r="J29" s="2">
+      <c r="P29" s="1">
         <v>1.5138619750909124</v>
       </c>
-      <c r="K29" s="33">
+      <c r="Q29" s="27">
         <v>0.14126823673653088</v>
       </c>
-      <c r="L29" s="2">
+      <c r="R29" s="1">
         <v>-0.73575873976904793</v>
       </c>
-      <c r="M29" s="2">
+      <c r="S29" s="1">
         <v>4.9031790004156388</v>
       </c>
-      <c r="N29" s="2">
+      <c r="T29" s="1">
         <v>-0.73575873976904793</v>
       </c>
-      <c r="O29" s="2">
+      <c r="U29" s="1">
         <v>4.9031790004156388</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>264</v>
       </c>
@@ -5190,16 +5454,24 @@
       <c r="D30">
         <v>15.8</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="10">
         <f t="shared" si="0"/>
         <v>17.067117539775701</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="10">
         <f t="shared" si="1"/>
         <v>-1.2671175397757004</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G30" s="10">
+        <v>1.6055868596072238</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>175</v>
       </c>
@@ -5212,19 +5484,27 @@
       <c r="D31">
         <v>19.7</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="10">
         <f t="shared" si="0"/>
         <v>21.554154315149582</v>
       </c>
-      <c r="F31" s="13">
+      <c r="F31" s="10">
         <f t="shared" si="1"/>
         <v>-1.8541543151495823</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="G31" s="10">
+        <v>3.4378882243878164</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>335</v>
       </c>
@@ -5237,16 +5517,24 @@
       <c r="D32">
         <v>15</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="10">
         <f t="shared" si="0"/>
         <v>13.254697831562694</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="10">
         <f t="shared" si="1"/>
         <v>1.7453021684373056</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G32" s="10">
+        <v>3.0460796591519608</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>109</v>
       </c>
@@ -5259,73 +5547,93 @@
       <c r="D33">
         <v>21.4</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="10">
         <f t="shared" si="0"/>
         <v>23.998964473934734</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="10">
         <f t="shared" si="1"/>
         <v>-2.5989644739347355</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="10">
+        <v>6.7546163367748564</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="J33" s="16" t="s">
+      <c r="P33" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F34" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G34" t="s">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" t="s">
         <v>3</v>
       </c>
-      <c r="H34">
+      <c r="N34">
         <v>200</v>
       </c>
-      <c r="J34" t="s">
+      <c r="P34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F35" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G35" s="30" t="s">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" t="s">
         <v>5</v>
       </c>
-      <c r="H35">
+      <c r="N35">
         <v>3.5</v>
       </c>
-      <c r="J35" t="s">
+      <c r="P35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F36" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="30" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" t="s">
         <v>8</v>
       </c>
-      <c r="H36">
+      <c r="N36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="F37" s="13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="30" t="s">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" t="s">
         <v>48</v>
       </c>
-      <c r="H37" s="31">
-        <f>H26+(H27*H34)+(H35*H28)+(H29*H36)</f>
+      <c r="N37" s="25">
+        <f>N26+(N27*N34)+(N35*N28)+(N29*N36)</f>
         <v>18.515826114235786</v>
       </c>
     </row>

</xml_diff>